<commit_message>
Deploying to master from  @ 482fc1c5ae4d3ae76d0e798229f3429888eb11bd 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_8-1-1.xlsx
+++ b/assets/excel/2021_8-1-1.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
-  <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hannover\Dez15-Uebergreifende-Analysen\Projekte\Integrationsmonitoring_2021\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\LSN\MT_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9074EA85-23FA-45BE-B0E2-D2B86384DE27}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="14010" xr2:uid="{3ED27CCD-7831-47CD-9649-40DDA4FF2B68}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="25">
   <si>
     <t>Migration und Teilhabe in Niedersachsen - Integrationsmonitoring 2021</t>
   </si>
@@ -102,21 +101,18 @@
   <si>
     <t>https://www.destatis.de/DE/Themen/Gesellschaft-Umwelt/Bevoelkerung/Haushalte-Familien/Methoden/mikrozensus-2020.html</t>
   </si>
-  <si>
-    <t>3) Die Ergebnisse des Mikrozensus 2020 sind unter anderem aufgrund methodischer Effekte im Rahmen einer Neugestaltung der Erhebung sowie insbesondere aufgrund der Folgen der Corona-Pandemie in Ihrer Datenqualität eingeschränkt. Auf die Verwendung dieser Ergebnisse wird daher verzichtet. Weitere Informationen zur methodischen Neugestaltung des Mikrozensus ab 2020 und zu den Auswirkungen der Neugestaltung und der Corona-Krise auf die Ergebnisse des Jahres 2020 finden Sie auf der Informationsseite des Statistischen Bundesamtes:</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#\ ###\ ###"/>
     <numFmt numFmtId="165" formatCode="###\ ##0"/>
     <numFmt numFmtId="166" formatCode="[&lt;5]&quot;-&quot;;[&lt;10]\(0.0\);#\ ###.0"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -352,7 +348,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -478,9 +474,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -525,9 +518,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Link 2" xfId="2" xr:uid="{8C712CB7-A698-4BFB-A344-D805BA2D57AA}"/>
+    <cellStyle name="Link 2" xfId="2"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard_Tabelle_A_6_HT" xfId="1" xr:uid="{2CFE44AD-1037-4D6A-B68D-718D552FDBB1}"/>
+    <cellStyle name="Standard_Tabelle_A_6_HT" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -838,27 +831,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F150A0D7-5577-4BEA-A4C0-1815A7A8D6E5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="B1:L191"/>
+  <dimension ref="B1:L190"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58:J58"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.7109375" style="31" customWidth="1"/>
     <col min="2" max="16384" width="11.42578125" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" customFormat="1">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:12" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" customFormat="1"/>
+    <row r="3" spans="2:12" customFormat="1">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -872,7 +863,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" s="7" customFormat="1">
       <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
@@ -886,7 +877,7 @@
       <c r="J4" s="5"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="2:12" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" s="7" customFormat="1" ht="8.25" customHeight="1">
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -898,29 +889,29 @@
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="6" spans="2:12" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="46" t="s">
+    <row r="6" spans="2:12" s="10" customFormat="1" ht="16.5" customHeight="1">
+      <c r="B6" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="57" t="s">
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
     </row>
-    <row r="7" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="47"/>
-      <c r="C7" s="50"/>
+    <row r="7" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1">
+      <c r="B7" s="46"/>
+      <c r="C7" s="49"/>
       <c r="D7" s="11" t="s">
         <v>6</v>
       </c>
@@ -942,23 +933,23 @@
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
     </row>
-    <row r="8" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="48"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="53" t="s">
+    <row r="8" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1">
+      <c r="B8" s="47"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="55" t="s">
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="56"/>
-      <c r="I8" s="56"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
     </row>
-    <row r="9" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B9" s="14">
         <v>1</v>
       </c>
@@ -985,7 +976,7 @@
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
     </row>
-    <row r="10" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B10" s="19" t="s">
         <v>11</v>
       </c>
@@ -1013,7 +1004,7 @@
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
     </row>
-    <row r="11" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B11" s="19" t="s">
         <v>12</v>
       </c>
@@ -1041,7 +1032,7 @@
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
     </row>
-    <row r="12" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B12" s="19" t="s">
         <v>13</v>
       </c>
@@ -1069,7 +1060,7 @@
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
     </row>
-    <row r="13" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B13" s="19" t="s">
         <v>14</v>
       </c>
@@ -1097,7 +1088,7 @@
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
     </row>
-    <row r="14" spans="2:12" s="36" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" s="36" customFormat="1" ht="16.5" customHeight="1">
       <c r="B14" s="38" t="s">
         <v>8</v>
       </c>
@@ -1125,7 +1116,7 @@
       <c r="J14" s="35"/>
       <c r="K14" s="35"/>
     </row>
-    <row r="15" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B15" s="15" t="s">
         <v>11</v>
       </c>
@@ -1153,7 +1144,7 @@
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
     </row>
-    <row r="16" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B16" s="15" t="s">
         <v>12</v>
       </c>
@@ -1181,7 +1172,7 @@
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
     </row>
-    <row r="17" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B17" s="15" t="s">
         <v>13</v>
       </c>
@@ -1209,7 +1200,7 @@
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
     </row>
-    <row r="18" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B18" s="15" t="s">
         <v>14</v>
       </c>
@@ -1237,7 +1228,7 @@
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
     </row>
-    <row r="19" spans="2:11" s="36" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" s="36" customFormat="1" ht="16.5" customHeight="1">
       <c r="B19" s="32" t="s">
         <v>8</v>
       </c>
@@ -1265,7 +1256,7 @@
       <c r="J19" s="35"/>
       <c r="K19" s="35"/>
     </row>
-    <row r="20" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B20" s="15" t="s">
         <v>11</v>
       </c>
@@ -1293,7 +1284,7 @@
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
     </row>
-    <row r="21" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B21" s="15" t="s">
         <v>12</v>
       </c>
@@ -1321,7 +1312,7 @@
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
     </row>
-    <row r="22" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B22" s="15" t="s">
         <v>13</v>
       </c>
@@ -1349,7 +1340,7 @@
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
     </row>
-    <row r="23" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B23" s="15" t="s">
         <v>14</v>
       </c>
@@ -1377,7 +1368,7 @@
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
     </row>
-    <row r="24" spans="2:11" s="36" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" s="36" customFormat="1" ht="16.5" customHeight="1">
       <c r="B24" s="32" t="s">
         <v>8</v>
       </c>
@@ -1405,7 +1396,7 @@
       <c r="J24" s="35"/>
       <c r="K24" s="35"/>
     </row>
-    <row r="25" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B25" s="15" t="s">
         <v>11</v>
       </c>
@@ -1433,7 +1424,7 @@
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
     </row>
-    <row r="26" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B26" s="15" t="s">
         <v>12</v>
       </c>
@@ -1461,7 +1452,7 @@
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
     </row>
-    <row r="27" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B27" s="15" t="s">
         <v>13</v>
       </c>
@@ -1489,7 +1480,7 @@
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
     </row>
-    <row r="28" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B28" s="15" t="s">
         <v>14</v>
       </c>
@@ -1517,7 +1508,7 @@
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
     </row>
-    <row r="29" spans="2:11" s="36" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" s="36" customFormat="1" ht="16.5" customHeight="1">
       <c r="B29" s="32" t="s">
         <v>8</v>
       </c>
@@ -1545,7 +1536,7 @@
       <c r="J29" s="35"/>
       <c r="K29" s="35"/>
     </row>
-    <row r="30" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B30" s="15" t="s">
         <v>11</v>
       </c>
@@ -1573,7 +1564,7 @@
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
     </row>
-    <row r="31" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B31" s="15" t="s">
         <v>12</v>
       </c>
@@ -1601,7 +1592,7 @@
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
     </row>
-    <row r="32" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B32" s="15" t="s">
         <v>13</v>
       </c>
@@ -1629,7 +1620,7 @@
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
     </row>
-    <row r="33" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B33" s="15" t="s">
         <v>14</v>
       </c>
@@ -1657,7 +1648,7 @@
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
     </row>
-    <row r="34" spans="2:11" s="36" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" s="36" customFormat="1" ht="16.5" customHeight="1">
       <c r="B34" s="32" t="s">
         <v>8</v>
       </c>
@@ -1685,7 +1676,7 @@
       <c r="J34" s="35"/>
       <c r="K34" s="35"/>
     </row>
-    <row r="35" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B35" s="15" t="s">
         <v>11</v>
       </c>
@@ -1713,7 +1704,7 @@
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
     </row>
-    <row r="36" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B36" s="15" t="s">
         <v>12</v>
       </c>
@@ -1741,7 +1732,7 @@
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
     </row>
-    <row r="37" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B37" s="15" t="s">
         <v>13</v>
       </c>
@@ -1769,7 +1760,7 @@
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
     </row>
-    <row r="38" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B38" s="15" t="s">
         <v>14</v>
       </c>
@@ -1797,7 +1788,7 @@
       <c r="J38" s="9"/>
       <c r="K38" s="9"/>
     </row>
-    <row r="39" spans="2:11" s="36" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11" s="36" customFormat="1" ht="16.5" customHeight="1">
       <c r="B39" s="32" t="s">
         <v>8</v>
       </c>
@@ -1825,7 +1816,7 @@
       <c r="J39" s="35"/>
       <c r="K39" s="35"/>
     </row>
-    <row r="40" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B40" s="15" t="s">
         <v>11</v>
       </c>
@@ -1853,7 +1844,7 @@
       <c r="J40" s="9"/>
       <c r="K40" s="9"/>
     </row>
-    <row r="41" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B41" s="15" t="s">
         <v>12</v>
       </c>
@@ -1881,7 +1872,7 @@
       <c r="J41" s="9"/>
       <c r="K41" s="9"/>
     </row>
-    <row r="42" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B42" s="15" t="s">
         <v>13</v>
       </c>
@@ -1909,7 +1900,7 @@
       <c r="J42" s="9"/>
       <c r="K42" s="9"/>
     </row>
-    <row r="43" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B43" s="15" t="s">
         <v>14</v>
       </c>
@@ -1937,7 +1928,7 @@
       <c r="J43" s="9"/>
       <c r="K43" s="9"/>
     </row>
-    <row r="44" spans="2:11" s="36" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:11" s="36" customFormat="1" ht="16.5" customHeight="1">
       <c r="B44" s="32" t="s">
         <v>8</v>
       </c>
@@ -1965,7 +1956,7 @@
       <c r="J44" s="35"/>
       <c r="K44" s="35"/>
     </row>
-    <row r="45" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B45" s="15" t="s">
         <v>11</v>
       </c>
@@ -1993,7 +1984,7 @@
       <c r="J45" s="9"/>
       <c r="K45" s="9"/>
     </row>
-    <row r="46" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B46" s="15" t="s">
         <v>12</v>
       </c>
@@ -2021,7 +2012,7 @@
       <c r="J46" s="9"/>
       <c r="K46" s="9"/>
     </row>
-    <row r="47" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B47" s="15" t="s">
         <v>13</v>
       </c>
@@ -2049,7 +2040,7 @@
       <c r="J47" s="9"/>
       <c r="K47" s="9"/>
     </row>
-    <row r="48" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B48" s="15" t="s">
         <v>14</v>
       </c>
@@ -2077,7 +2068,7 @@
       <c r="J48" s="9"/>
       <c r="K48" s="9"/>
     </row>
-    <row r="49" spans="2:11" s="36" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11" s="36" customFormat="1" ht="16.5" customHeight="1">
       <c r="B49" s="32" t="s">
         <v>8</v>
       </c>
@@ -2105,7 +2096,7 @@
       <c r="J49" s="35"/>
       <c r="K49" s="35"/>
     </row>
-    <row r="50" spans="2:11" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:11" s="7" customFormat="1" ht="8.25" customHeight="1">
       <c r="B50" s="15" t="s">
         <v>11</v>
       </c>
@@ -2133,7 +2124,7 @@
       <c r="J50" s="8"/>
       <c r="K50" s="8"/>
     </row>
-    <row r="51" spans="2:11" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11" s="7" customFormat="1" ht="8.25" customHeight="1">
       <c r="B51" s="15" t="s">
         <v>12</v>
       </c>
@@ -2161,7 +2152,7 @@
       <c r="J51" s="8"/>
       <c r="K51" s="8"/>
     </row>
-    <row r="52" spans="2:11" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11" s="7" customFormat="1" ht="8.25" customHeight="1">
       <c r="B52" s="15" t="s">
         <v>13</v>
       </c>
@@ -2189,7 +2180,7 @@
       <c r="J52" s="8"/>
       <c r="K52" s="8"/>
     </row>
-    <row r="53" spans="2:11" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11" s="7" customFormat="1" ht="8.25" customHeight="1">
       <c r="B53" s="15" t="s">
         <v>14</v>
       </c>
@@ -2217,7 +2208,7 @@
       <c r="J53" s="8"/>
       <c r="K53" s="8"/>
     </row>
-    <row r="54" spans="2:11" s="41" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:11" s="41" customFormat="1" ht="16.5" customHeight="1">
       <c r="B54" s="32" t="s">
         <v>8</v>
       </c>
@@ -2245,7 +2236,7 @@
       <c r="J54" s="40"/>
       <c r="K54" s="40"/>
     </row>
-    <row r="55" spans="2:11" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:11" s="7" customFormat="1" ht="8.25" customHeight="1">
       <c r="B55" s="21"/>
       <c r="C55" s="21"/>
       <c r="D55" s="22"/>
@@ -2257,7 +2248,7 @@
       <c r="J55" s="8"/>
       <c r="K55" s="8"/>
     </row>
-    <row r="56" spans="2:11" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:11" s="7" customFormat="1" ht="8.25" customHeight="1">
       <c r="B56" s="24"/>
       <c r="C56" s="25"/>
       <c r="D56" s="26"/>
@@ -2269,65 +2260,64 @@
       <c r="J56" s="8"/>
       <c r="K56" s="8"/>
     </row>
-    <row r="57" spans="2:11" s="27" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="45" t="s">
+    <row r="57" spans="2:11" s="27" customFormat="1" ht="24.75" customHeight="1">
+      <c r="B57" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="C57" s="45"/>
-      <c r="D57" s="45"/>
-      <c r="E57" s="45"/>
-      <c r="F57" s="45"/>
-      <c r="G57" s="45"/>
-      <c r="H57" s="45"/>
-      <c r="I57" s="45"/>
-      <c r="J57" s="45"/>
+      <c r="C57" s="44"/>
+      <c r="D57" s="44"/>
+      <c r="E57" s="44"/>
+      <c r="F57" s="44"/>
+      <c r="G57" s="44"/>
+      <c r="H57" s="44"/>
+      <c r="I57" s="44"/>
+      <c r="J57" s="44"/>
       <c r="K57" s="8"/>
     </row>
-    <row r="58" spans="2:11" s="27" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="45" t="s">
+    <row r="58" spans="2:11" s="27" customFormat="1" ht="24.75" customHeight="1">
+      <c r="B58" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="C58" s="45"/>
-      <c r="D58" s="45"/>
-      <c r="E58" s="45"/>
-      <c r="F58" s="45"/>
-      <c r="G58" s="45"/>
-      <c r="H58" s="45"/>
-      <c r="I58" s="45"/>
-      <c r="J58" s="45"/>
+      <c r="C58" s="44"/>
+      <c r="D58" s="44"/>
+      <c r="E58" s="44"/>
+      <c r="F58" s="44"/>
+      <c r="G58" s="44"/>
+      <c r="H58" s="44"/>
+      <c r="I58" s="44"/>
+      <c r="J58" s="44"/>
       <c r="K58" s="8"/>
     </row>
-    <row r="59" spans="2:11" s="27" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="C59" s="44"/>
-      <c r="D59" s="44"/>
-      <c r="E59" s="44"/>
-      <c r="F59" s="44"/>
-      <c r="G59" s="44"/>
-      <c r="H59" s="44"/>
-      <c r="I59" s="44"/>
-      <c r="J59" s="44"/>
+    <row r="59" spans="2:11" s="27" customFormat="1" ht="8.25" customHeight="1">
+      <c r="B59" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="9"/>
+      <c r="H59" s="9"/>
+      <c r="I59" s="9"/>
+      <c r="J59" s="42"/>
       <c r="K59" s="8"/>
     </row>
-    <row r="60" spans="2:11" s="27" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="C60" s="9"/>
-      <c r="D60" s="9"/>
-      <c r="E60" s="9"/>
-      <c r="F60" s="9"/>
-      <c r="G60" s="9"/>
-      <c r="H60" s="9"/>
-      <c r="I60" s="9"/>
-      <c r="J60" s="42"/>
-      <c r="K60" s="8"/>
-    </row>
-    <row r="61" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="28"/>
-      <c r="C61" s="28"/>
+    <row r="60" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1">
+      <c r="B60" s="28"/>
+      <c r="C60" s="28"/>
+      <c r="D60" s="29"/>
+      <c r="E60" s="29"/>
+      <c r="F60" s="29"/>
+      <c r="G60" s="29"/>
+      <c r="H60" s="29"/>
+      <c r="I60" s="29"/>
+      <c r="J60" s="29"/>
+    </row>
+    <row r="61" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1">
+      <c r="B61" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C61" s="30"/>
       <c r="D61" s="29"/>
       <c r="E61" s="29"/>
       <c r="F61" s="29"/>
@@ -2336,163 +2326,161 @@
       <c r="I61" s="29"/>
       <c r="J61" s="29"/>
     </row>
-    <row r="62" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="C62" s="30"/>
-      <c r="D62" s="29"/>
-      <c r="E62" s="29"/>
-      <c r="F62" s="29"/>
-      <c r="G62" s="29"/>
-      <c r="H62" s="29"/>
-      <c r="I62" s="29"/>
-      <c r="J62" s="29"/>
-    </row>
-    <row r="63" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1"/>
+    <row r="63" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1">
+      <c r="B63" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64" spans="2:11" s="10" customFormat="1" ht="8.25" customHeight="1">
       <c r="B64" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="65" spans="2:2" s="10" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" s="10" customFormat="1" ht="8.25">
       <c r="B65" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="66" spans="2:2" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" s="10" customFormat="1" ht="8.25">
       <c r="B66" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="67" spans="2:2" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25">
-      <c r="B67" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="2:2" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="2:2" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="70" spans="2:2" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="2:2" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="72" spans="2:2" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="2:2" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="2:2" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="2:2" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="76" spans="2:2" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="2:2" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="2:2" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="2:2" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="2:2" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="81" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="82" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="83" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="84" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="85" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="86" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="87" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="88" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="89" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="90" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="91" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="92" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="93" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="94" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="95" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="96" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="97" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="98" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="99" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="100" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="101" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="102" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="103" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="104" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="105" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="106" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="107" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="108" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="109" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="110" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="111" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="112" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="113" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="114" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="115" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="116" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="117" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="118" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="119" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="120" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="121" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="122" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="123" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="124" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="125" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="126" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="127" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="128" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="129" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="130" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="131" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="132" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="133" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="134" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="135" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="136" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="137" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="138" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="139" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="140" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="141" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="142" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="143" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="144" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="145" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="146" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="147" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="148" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="149" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="150" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="151" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="152" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="153" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="154" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="155" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="156" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="157" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="158" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="159" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="160" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="161" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="162" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="163" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="164" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="165" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="166" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="167" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="168" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="169" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="170" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="171" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="172" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="173" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="174" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="175" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="176" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="177" spans="2:10" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="178" spans="2:10" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="179" spans="2:10" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="180" spans="2:10" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="181" spans="2:10" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="182" spans="2:10" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="183" spans="2:10" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="184" spans="2:10" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="185" spans="2:10" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="186" spans="2:10" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="187" spans="2:10" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="188" spans="2:10" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="189" spans="2:10" s="10" customFormat="1" ht="8.25" x14ac:dyDescent="0.25"/>
-    <row r="190" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:2" s="10" customFormat="1" ht="8.25"/>
+    <row r="68" spans="2:2" s="10" customFormat="1" ht="8.25"/>
+    <row r="69" spans="2:2" s="10" customFormat="1" ht="8.25"/>
+    <row r="70" spans="2:2" s="10" customFormat="1" ht="8.25"/>
+    <row r="71" spans="2:2" s="10" customFormat="1" ht="8.25"/>
+    <row r="72" spans="2:2" s="10" customFormat="1" ht="8.25"/>
+    <row r="73" spans="2:2" s="10" customFormat="1" ht="8.25"/>
+    <row r="74" spans="2:2" s="10" customFormat="1" ht="8.25"/>
+    <row r="75" spans="2:2" s="10" customFormat="1" ht="8.25"/>
+    <row r="76" spans="2:2" s="10" customFormat="1" ht="8.25"/>
+    <row r="77" spans="2:2" s="10" customFormat="1" ht="8.25"/>
+    <row r="78" spans="2:2" s="10" customFormat="1" ht="8.25"/>
+    <row r="79" spans="2:2" s="10" customFormat="1" ht="8.25"/>
+    <row r="80" spans="2:2" s="10" customFormat="1" ht="8.25"/>
+    <row r="81" s="10" customFormat="1" ht="8.25"/>
+    <row r="82" s="10" customFormat="1" ht="8.25"/>
+    <row r="83" s="10" customFormat="1" ht="8.25"/>
+    <row r="84" s="10" customFormat="1" ht="8.25"/>
+    <row r="85" s="10" customFormat="1" ht="8.25"/>
+    <row r="86" s="10" customFormat="1" ht="8.25"/>
+    <row r="87" s="10" customFormat="1" ht="8.25"/>
+    <row r="88" s="10" customFormat="1" ht="8.25"/>
+    <row r="89" s="10" customFormat="1" ht="8.25"/>
+    <row r="90" s="10" customFormat="1" ht="8.25"/>
+    <row r="91" s="10" customFormat="1" ht="8.25"/>
+    <row r="92" s="10" customFormat="1" ht="8.25"/>
+    <row r="93" s="10" customFormat="1" ht="8.25"/>
+    <row r="94" s="10" customFormat="1" ht="8.25"/>
+    <row r="95" s="10" customFormat="1" ht="8.25"/>
+    <row r="96" s="10" customFormat="1" ht="8.25"/>
+    <row r="97" s="10" customFormat="1" ht="8.25"/>
+    <row r="98" s="10" customFormat="1" ht="8.25"/>
+    <row r="99" s="10" customFormat="1" ht="8.25"/>
+    <row r="100" s="10" customFormat="1" ht="8.25"/>
+    <row r="101" s="10" customFormat="1" ht="8.25"/>
+    <row r="102" s="10" customFormat="1" ht="8.25"/>
+    <row r="103" s="10" customFormat="1" ht="8.25"/>
+    <row r="104" s="10" customFormat="1" ht="8.25"/>
+    <row r="105" s="10" customFormat="1" ht="8.25"/>
+    <row r="106" s="10" customFormat="1" ht="8.25"/>
+    <row r="107" s="10" customFormat="1" ht="8.25"/>
+    <row r="108" s="10" customFormat="1" ht="8.25"/>
+    <row r="109" s="10" customFormat="1" ht="8.25"/>
+    <row r="110" s="10" customFormat="1" ht="8.25"/>
+    <row r="111" s="10" customFormat="1" ht="8.25"/>
+    <row r="112" s="10" customFormat="1" ht="8.25"/>
+    <row r="113" s="10" customFormat="1" ht="8.25"/>
+    <row r="114" s="10" customFormat="1" ht="8.25"/>
+    <row r="115" s="10" customFormat="1" ht="8.25"/>
+    <row r="116" s="10" customFormat="1" ht="8.25"/>
+    <row r="117" s="10" customFormat="1" ht="8.25"/>
+    <row r="118" s="10" customFormat="1" ht="8.25"/>
+    <row r="119" s="10" customFormat="1" ht="8.25"/>
+    <row r="120" s="10" customFormat="1" ht="8.25"/>
+    <row r="121" s="10" customFormat="1" ht="8.25"/>
+    <row r="122" s="10" customFormat="1" ht="8.25"/>
+    <row r="123" s="10" customFormat="1" ht="8.25"/>
+    <row r="124" s="10" customFormat="1" ht="8.25"/>
+    <row r="125" s="10" customFormat="1" ht="8.25"/>
+    <row r="126" s="10" customFormat="1" ht="8.25"/>
+    <row r="127" s="10" customFormat="1" ht="8.25"/>
+    <row r="128" s="10" customFormat="1" ht="8.25"/>
+    <row r="129" s="10" customFormat="1" ht="8.25"/>
+    <row r="130" s="10" customFormat="1" ht="8.25"/>
+    <row r="131" s="10" customFormat="1" ht="8.25"/>
+    <row r="132" s="10" customFormat="1" ht="8.25"/>
+    <row r="133" s="10" customFormat="1" ht="8.25"/>
+    <row r="134" s="10" customFormat="1" ht="8.25"/>
+    <row r="135" s="10" customFormat="1" ht="8.25"/>
+    <row r="136" s="10" customFormat="1" ht="8.25"/>
+    <row r="137" s="10" customFormat="1" ht="8.25"/>
+    <row r="138" s="10" customFormat="1" ht="8.25"/>
+    <row r="139" s="10" customFormat="1" ht="8.25"/>
+    <row r="140" s="10" customFormat="1" ht="8.25"/>
+    <row r="141" s="10" customFormat="1" ht="8.25"/>
+    <row r="142" s="10" customFormat="1" ht="8.25"/>
+    <row r="143" s="10" customFormat="1" ht="8.25"/>
+    <row r="144" s="10" customFormat="1" ht="8.25"/>
+    <row r="145" s="10" customFormat="1" ht="8.25"/>
+    <row r="146" s="10" customFormat="1" ht="8.25"/>
+    <row r="147" s="10" customFormat="1" ht="8.25"/>
+    <row r="148" s="10" customFormat="1" ht="8.25"/>
+    <row r="149" s="10" customFormat="1" ht="8.25"/>
+    <row r="150" s="10" customFormat="1" ht="8.25"/>
+    <row r="151" s="10" customFormat="1" ht="8.25"/>
+    <row r="152" s="10" customFormat="1" ht="8.25"/>
+    <row r="153" s="10" customFormat="1" ht="8.25"/>
+    <row r="154" s="10" customFormat="1" ht="8.25"/>
+    <row r="155" s="10" customFormat="1" ht="8.25"/>
+    <row r="156" s="10" customFormat="1" ht="8.25"/>
+    <row r="157" s="10" customFormat="1" ht="8.25"/>
+    <row r="158" s="10" customFormat="1" ht="8.25"/>
+    <row r="159" s="10" customFormat="1" ht="8.25"/>
+    <row r="160" s="10" customFormat="1" ht="8.25"/>
+    <row r="161" s="10" customFormat="1" ht="8.25"/>
+    <row r="162" s="10" customFormat="1" ht="8.25"/>
+    <row r="163" s="10" customFormat="1" ht="8.25"/>
+    <row r="164" s="10" customFormat="1" ht="8.25"/>
+    <row r="165" s="10" customFormat="1" ht="8.25"/>
+    <row r="166" s="10" customFormat="1" ht="8.25"/>
+    <row r="167" s="10" customFormat="1" ht="8.25"/>
+    <row r="168" s="10" customFormat="1" ht="8.25"/>
+    <row r="169" s="10" customFormat="1" ht="8.25"/>
+    <row r="170" s="10" customFormat="1" ht="8.25"/>
+    <row r="171" s="10" customFormat="1" ht="8.25"/>
+    <row r="172" s="10" customFormat="1" ht="8.25"/>
+    <row r="173" s="10" customFormat="1" ht="8.25"/>
+    <row r="174" s="10" customFormat="1" ht="8.25"/>
+    <row r="175" s="10" customFormat="1" ht="8.25"/>
+    <row r="176" s="10" customFormat="1" ht="8.25"/>
+    <row r="177" spans="2:10" s="10" customFormat="1" ht="8.25"/>
+    <row r="178" spans="2:10" s="10" customFormat="1" ht="8.25"/>
+    <row r="179" spans="2:10" s="10" customFormat="1" ht="8.25"/>
+    <row r="180" spans="2:10" s="10" customFormat="1" ht="8.25"/>
+    <row r="181" spans="2:10" s="10" customFormat="1" ht="8.25"/>
+    <row r="182" spans="2:10" s="10" customFormat="1" ht="8.25"/>
+    <row r="183" spans="2:10" s="10" customFormat="1" ht="8.25"/>
+    <row r="184" spans="2:10" s="10" customFormat="1" ht="8.25"/>
+    <row r="185" spans="2:10" s="10" customFormat="1" ht="8.25"/>
+    <row r="186" spans="2:10" s="10" customFormat="1" ht="8.25"/>
+    <row r="187" spans="2:10" s="10" customFormat="1" ht="8.25"/>
+    <row r="188" spans="2:10" s="10" customFormat="1" ht="8.25"/>
+    <row r="189" spans="2:10">
+      <c r="B189" s="10"/>
+      <c r="C189" s="10"/>
+      <c r="D189" s="10"/>
+      <c r="E189" s="10"/>
+      <c r="F189" s="10"/>
+      <c r="G189" s="10"/>
+      <c r="H189" s="10"/>
+      <c r="I189" s="10"/>
+      <c r="J189" s="10"/>
+    </row>
+    <row r="190" spans="2:10">
       <c r="B190" s="10"/>
       <c r="C190" s="10"/>
       <c r="D190" s="10"/>
@@ -2503,23 +2491,11 @@
       <c r="I190" s="10"/>
       <c r="J190" s="10"/>
     </row>
-    <row r="191" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B191" s="10"/>
-      <c r="C191" s="10"/>
-      <c r="D191" s="10"/>
-      <c r="E191" s="10"/>
-      <c r="F191" s="10"/>
-      <c r="G191" s="10"/>
-      <c r="H191" s="10"/>
-      <c r="I191" s="10"/>
-      <c r="J191" s="10"/>
-    </row>
   </sheetData>
   <sortState ref="B10:I54">
     <sortCondition descending="1" ref="C10:C54"/>
   </sortState>
-  <mergeCells count="9">
-    <mergeCell ref="B59:J59"/>
+  <mergeCells count="8">
     <mergeCell ref="B58:J58"/>
     <mergeCell ref="B57:J57"/>
     <mergeCell ref="B6:B8"/>
@@ -2530,8 +2506,8 @@
     <mergeCell ref="G6:I6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B67" r:id="rId1" xr:uid="{0A153FDA-E3A9-4294-A2DC-B7CB53E079FE}"/>
-    <hyperlink ref="B60" r:id="rId2" xr:uid="{E22D1C72-2ECE-42DE-BDBB-9AEAA5D246DC}"/>
+    <hyperlink ref="B66" r:id="rId1"/>
+    <hyperlink ref="B59" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>